<commit_message>
Import Absen sudah oke, lanjut -> Pe Disicpline
</commit_message>
<xml_diff>
--- a/public/documents/discipline-assesment.xlsx
+++ b/public/documents/discipline-assesment.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">Bisnis Unit</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">Bulan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tahun</t>
   </si>
   <si>
     <t xml:space="preserve">NIK</t>
@@ -38,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">Terlambat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN-4-034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nurdiansah</t>
   </si>
 </sst>
 </file>
@@ -76,6 +85,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -95,14 +105,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDEE6EF"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -156,19 +166,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,27 +263,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="12.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="12.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="16.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -285,18 +295,30 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="n">
-        <v>0</v>
+      <c r="A2" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -307,6 +329,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
@@ -315,6 +338,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
@@ -323,6 +347,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
@@ -331,6 +356,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
@@ -339,6 +365,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
@@ -347,6 +374,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
@@ -355,6 +383,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
@@ -363,6 +392,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
@@ -371,6 +401,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
@@ -379,6 +410,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
@@ -387,6 +419,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
@@ -395,6 +428,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
@@ -403,6 +437,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
@@ -411,6 +446,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
@@ -419,6 +455,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
@@ -427,6 +464,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
@@ -435,6 +473,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
@@ -443,6 +482,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
@@ -451,6 +491,7 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>